<commit_message>
Update validators to be a series of validators called on the object you want to validate
</commit_message>
<xml_diff>
--- a/hedtools/tests/data/hed3_tags_single_sheet_bad_defs.xlsx
+++ b/hedtools/tests/data/hed3_tags_single_sheet_bad_defs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">Event code</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Awake, (Definition/Def1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Def/DefInvalid</t>
   </si>
 </sst>
 </file>
@@ -175,10 +178,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,8 +235,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>